<commit_message>
Update median and median with h2 ptc, fixed error in htse cashflows
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results_laptop.xlsx
+++ b/use_cases/LWRS/LWRS_results_laptop.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F789AF7-3E70-BE42-ABC9-3EC91EBD206A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FEEA42-FB11-3847-B8B8-9A71A5BD9F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1180" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$3</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -300,13 +286,13 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-1061861758.29</c:v>
+                  <c:v>-341968587.97000027</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2059652734.5499997</c:v>
+                  <c:v>-1339759564.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1324074290.1499996</c:v>
+                  <c:v>-604181119.82999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,13 +371,13 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1153391085.3199997</c:v>
+                  <c:v>1873284255.6399994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2057933596.8400002</c:v>
+                  <c:v>2777826767.1599998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2763364635.6700001</c:v>
+                  <c:v>3483257805.9899998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,7 +674,7 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1359469130.8699999</c:v>
+                  <c:v>639575960.55000019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,7 +874,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
-          <c:builtInUnit val="billions"/>
+          <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -2437,7 +2423,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,26 +2490,26 @@
         <v>23</v>
       </c>
       <c r="B3" s="2">
-        <v>5268073350.6599998</v>
+        <v>4548180180.3400002</v>
       </c>
       <c r="C3" s="2">
-        <v>7474182.8462399999</v>
+        <v>6798603.1220399998</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D10" si="0">C3/B3</f>
-        <v>1.4187696997999492E-3</v>
+        <v>1.4947963476530011E-3</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E10" si="1">B3-$B$2</f>
-        <v>1359469130.8699999</v>
+        <v>639575960.55000019</v>
       </c>
       <c r="F3" s="2">
         <f>SQRT(POWER($C$2,2)+POWER(C3,2))</f>
-        <v>12570709.75914102</v>
+        <v>12181146.868852172</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G10" si="2">ABS(F3/E3)</f>
-        <v>9.2467783737732422E-3</v>
+        <v>1.9045660906918789E-2</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -2534,10 +2520,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="2">
-        <v>3638324134.23</v>
+        <v>6178525094.7600002</v>
       </c>
       <c r="C4" s="2">
-        <v>10614260.6822</v>
+        <v>4320401.8213999998</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
@@ -2729,19 +2715,19 @@
       </c>
       <c r="B13" s="2">
         <f>E5-E3</f>
-        <v>-1061861758.29</v>
+        <v>-341968587.97000027</v>
       </c>
       <c r="C13" s="2">
         <f>E6-E3</f>
-        <v>1153391085.3199997</v>
+        <v>1873284255.6399994</v>
       </c>
       <c r="D13" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F5,2))</f>
-        <v>16130160.522390913</v>
+        <v>15828445.080616167</v>
       </c>
       <c r="E13" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F6,2))</f>
-        <v>16130160.522390913</v>
+        <v>15828445.080616167</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2750,19 +2736,19 @@
       </c>
       <c r="B14" s="2">
         <f>E7-E3</f>
-        <v>-2059652734.5499997</v>
+        <v>-1339759564.23</v>
       </c>
       <c r="C14" s="2">
         <f>E8-E3</f>
-        <v>2057933596.8400002</v>
+        <v>2777826767.1599998</v>
       </c>
       <c r="D14" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F7,2))</f>
-        <v>17299703.275359429</v>
+        <v>17018734.635908321</v>
       </c>
       <c r="E14" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F8,2))</f>
-        <v>18205846.528829522</v>
+        <v>17939075.868708447</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2771,19 +2757,19 @@
       </c>
       <c r="B15" s="2">
         <f>E9-E3</f>
-        <v>-1324074290.1499996</v>
+        <v>-604181119.82999992</v>
       </c>
       <c r="C15" s="2">
         <f>E10-E3</f>
-        <v>2763364635.6700001</v>
+        <v>3483257805.9899998</v>
       </c>
       <c r="D15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F9,2))</f>
-        <v>19041252.56443315</v>
+        <v>18786348.618465371</v>
       </c>
       <c r="E15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F10,2))</f>
-        <v>16130160.522390913</v>
+        <v>15828445.080616167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results after fixing mistake in HTSE cashflows
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results_laptop.xlsx
+++ b/use_cases/LWRS/LWRS_results_laptop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FEEA42-FB11-3847-B8B8-9A71A5BD9F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F0589-65B2-A840-B848-29BB26CAA935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1180" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="-36260" yWindow="940" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,27 @@
     <t>Ref for SA</t>
   </si>
   <si>
-    <t>Median H2 PTC</t>
+    <r>
+      <t>Median H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PTC</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -126,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +160,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,9 +273,44 @@
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1000000000"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
@@ -286,13 +346,13 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-341968587.97000027</c:v>
+                  <c:v>-1063205222.8900003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1339759564.23</c:v>
+                  <c:v>-2061486996.0799999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-604181119.82999992</c:v>
+                  <c:v>-790038144.14000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,9 +393,44 @@
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1000000000"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$13:$E$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17258366.63144559</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$13:$D$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>15828445.080616167</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>17190871.780215744</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18919850.81651184</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
@@ -371,13 +466,13 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1873284255.6399994</c:v>
+                  <c:v>1152047620.7200003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2777826767.1599998</c:v>
+                  <c:v>2055019080.4700003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3483257805.9899998</c:v>
+                  <c:v>5770030407.7600002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,8 +551,8 @@
         <c:axId val="689775903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4000000000"/>
-          <c:min val="-4000000000"/>
+          <c:max val="6000000000"/>
+          <c:min val="-3000000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -512,7 +607,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000000000"/>
-        <c:minorUnit val="500000000"/>
+        <c:minorUnit val="250000000"/>
         <c:dispUnits>
           <c:builtInUnit val="billions"/>
           <c:dispUnitsLbl>
@@ -642,9 +737,38 @@
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="12570709.76"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
@@ -658,23 +782,29 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$3:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Median</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Median H2 PTC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3</c:f>
+              <c:f>Sheet1!$E$3:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>639575960.55000019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2269920874.9700003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,14 +2181,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>878417</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>65617</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>3527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>730250</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2086,16 +2216,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>963084</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>196849</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>137583</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2422,14 +2552,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
@@ -2525,28 +2655,40 @@
       <c r="C4" s="2">
         <v>4320401.8213999998</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.9926102996071464E-4</v>
+      </c>
+      <c r="E4" s="2">
+        <f>B4-$B$2</f>
+        <v>2269920874.9700003</v>
+      </c>
+      <c r="F4" s="2">
+        <f>SQRT(POWER($C$2,2)+POWER(C4,2))</f>
+        <v>10992051.970760122</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="2"/>
+        <v>4.8424824371490023E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>4206211592.3699999</v>
+        <v>3484974957.4499998</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>5.0263049764099996E-7</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4422786498551515E-16</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>297607372.57999992</v>
+        <v>-423629262.34000015</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ref="F5:F10" si="3">SQRT(POWER($C$2,2)+POWER(C5,2))</f>
@@ -2554,7 +2696,7 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>3.3962163007514305E-2</v>
+        <v>2.3859046100757602E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2562,18 +2704,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>6421464435.9799995</v>
+        <v>5700227801.0600004</v>
       </c>
       <c r="C6" s="2">
         <v>1.96215910359E-6</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>3.0556255868923904E-16</v>
+        <v>3.4422468225307095E-16</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>2512860216.1899996</v>
+        <v>1791623581.2700005</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="3"/>
@@ -2581,7 +2723,7 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="2"/>
-        <v>4.0222651601070081E-3</v>
+        <v>5.6414696733536685E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2589,26 +2731,26 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3208420616.1100001</v>
+        <v>2486693184.2600002</v>
       </c>
       <c r="C7" s="2">
-        <v>6252811.7625099998</v>
+        <v>6707190.08928</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>1.9488753223669047E-3</v>
+        <v>2.6972326669548303E-3</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>-700183603.67999983</v>
+        <v>-1421911035.5299997</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>11885158.373657392</v>
+        <v>12130364.113383856</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="2"/>
-        <v>1.6974345459093591E-2</v>
+        <v>8.5310288831554164E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2616,26 +2758,26 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>7326006947.5</v>
+        <v>6603199260.8100004</v>
       </c>
       <c r="C8" s="2">
-        <v>8442201.6887299996</v>
+        <v>6878338.8339999998</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>1.1523605900497953E-3</v>
+        <v>1.0416676163057736E-3</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>3417402727.71</v>
+        <v>2694595041.0200005</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>13169286.388515161</v>
+        <v>12225828.386855736</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="2"/>
-        <v>3.853595094816318E-3</v>
+        <v>4.537167255465528E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2643,26 +2785,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>3943999060.5100002</v>
+        <v>3758142036.1999998</v>
       </c>
       <c r="C9" s="2">
-        <v>10118657.0623</v>
+        <v>10364414.1778</v>
       </c>
       <c r="D9" s="1">
         <f>C9/B9</f>
-        <v>2.5655830305881342E-3</v>
+        <v>2.7578558973997301E-3</v>
       </c>
       <c r="E9" s="2">
         <f>B9-$B$2</f>
-        <v>35394840.720000267</v>
+        <v>-150462183.59000015</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="3"/>
-        <v>14301977.323921638</v>
+        <v>14476892.480035786</v>
       </c>
       <c r="G9" s="1">
         <f>ABS(F9/E9)</f>
-        <v>0.40406954892270891</v>
+        <v>9.6216153020112966E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2670,18 +2812,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>8031437986.3299999</v>
+        <v>10318210588.1</v>
       </c>
       <c r="C10" s="2">
-        <v>9.7844920357199997E-7</v>
+        <v>3.8799104897699997E-6</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>1.2182739943175563E-16</v>
+        <v>3.7602551882830375E-16</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>4122833766.54</v>
+        <v>6409606368.3100004</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
@@ -2689,8 +2831,11 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="2"/>
-        <v>2.4515638204550775E-3</v>
-      </c>
+        <v>1.5769127648419044E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2715,11 +2860,11 @@
       </c>
       <c r="B13" s="2">
         <f>E5-E3</f>
-        <v>-341968587.97000027</v>
+        <v>-1063205222.8900003</v>
       </c>
       <c r="C13" s="2">
         <f>E6-E3</f>
-        <v>1873284255.6399994</v>
+        <v>1152047620.7200003</v>
       </c>
       <c r="D13" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F5,2))</f>
@@ -2736,19 +2881,19 @@
       </c>
       <c r="B14" s="2">
         <f>E7-E3</f>
-        <v>-1339759564.23</v>
+        <v>-2061486996.0799999</v>
       </c>
       <c r="C14" s="2">
         <f>E8-E3</f>
-        <v>2777826767.1599998</v>
+        <v>2055019080.4700003</v>
       </c>
       <c r="D14" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F7,2))</f>
-        <v>17018734.635908321</v>
+        <v>17190871.780215744</v>
       </c>
       <c r="E14" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F8,2))</f>
-        <v>17939075.868708447</v>
+        <v>17258366.63144559</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2757,15 +2902,15 @@
       </c>
       <c r="B15" s="2">
         <f>E9-E3</f>
-        <v>-604181119.82999992</v>
+        <v>-790038144.14000034</v>
       </c>
       <c r="C15" s="2">
         <f>E10-E3</f>
-        <v>3483257805.9899998</v>
+        <v>5770030407.7600002</v>
       </c>
       <c r="D15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F9,2))</f>
-        <v>18786348.618465371</v>
+        <v>18919850.81651184</v>
       </c>
       <c r="E15" s="2">
         <f>SQRT(POWER($F$3,2)+POWER(F10,2))</f>

</xml_diff>

<commit_message>
Modify training RAVEN input to print prediction
</commit_message>
<xml_diff>
--- a/use_cases/LWRS/LWRS_results_laptop.xlsx
+++ b/use_cases/LWRS/LWRS_results_laptop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWRS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F0589-65B2-A840-B848-29BB26CAA935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FD343-7083-8A46-9A21-671A218406E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36260" yWindow="940" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
+    <workbookView xWindow="0" yWindow="920" windowWidth="35840" windowHeight="19400" xr2:uid="{9EE474E5-2592-4044-A45A-603D647FE853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -588,7 +588,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1004,6 +1004,402 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean NPV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="64000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3:$F$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>12181146.868852172</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10992051.970760122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>639575960.55000019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3DA-1B4E-AA13-C7DD1AF36678}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:axId val="776062752"/>
+        <c:axId val="528268015"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="776062752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528268015"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528268015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Δ NPV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="776062752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
             <c:spPr>
@@ -1168,6 +1564,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -1674,6 +2110,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2245,6 +3184,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{029D3ADC-DB77-0944-9DCB-DF5DD35CE67F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2552,8 +3529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B72939-7718-F04D-9ED0-21E4DB6080A0}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>